<commit_message>
with json schema validation
</commit_message>
<xml_diff>
--- a/Spotify_API/src/test/resources/TestData/Data.xlsx
+++ b/Spotify_API/src/test/resources/TestData/Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="117">
   <si>
     <t>testCase</t>
   </si>
@@ -375,6 +375,9 @@
   </si>
   <si>
     <t>BQBrFedo6OQWFaqf1eRqBXwucGg9f0PRcCrY5sxN2mcsn5cRYs_zu3YhZOM1Lt5oVlJETI6qKay8gtbO6qEO_1CPlikWsAsjoueRVeDhpavkI0YfsKv1y1-hiEJXcuFHolP67rHFkUo_JOCdOGP2xFZyfhTQydkB8VfgAZIsqqqQ-4iCtlrOgvXvTDXvEDd00SqS92kjTFpKHLTZxgRm0wsp6U_PoOHthU2qHKz9OeZs_s24-UnuOJUqmbTX3hHiowQ6AHBD0sFpjet6jc9oP2HHtPGGPOlTAp1awwNwfqP98sgmvb-k62pc1EuywQryzZfJdLN5xI68uINK9CcZ</t>
+  </si>
+  <si>
+    <t>BQALLyim8w3kc4ZgsaMZ8ILIlZSuDaeIu8dcyEPWBnHEnhymHc-dp5DizVUcVlfW64El4kD1WeQ-DkBtCr2hVgi55lzBOcom-jVckOAzXTtPnDA32GOz9_xPgI1qv6SzFN-tdlHKJcD0xKMjRQhixiCPKtwMuc33tqkUimrJGcp80WIUXSaP61yKGmD8DegUsjKVB13iw6TIeVYsENWhhKBGYxFtN9ypWflI8WzlVkbtXfssBCpx8s1IbG0P4ffO2I6Qly8h4HmxihKZFNqV5_SW-pyHDkDlebOn9M_g8ogmwF382XjHNQZVc4tuviuPjNBVt1BaQ6gbnS_3RukU</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1053,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1068,13 +1071,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="9.140625" collapsed="false"/>
+    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="45.140625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="15.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="53.42578125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="53.42578125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="36.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="2" width="33.85546875" collapsed="false"/>
-    <col min="7" max="16384" style="2" width="9.140625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="2" width="33.85546875" collapsed="true"/>
+    <col min="7" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>